<commit_message>
medio performer hecho siuuuuu
</commit_message>
<xml_diff>
--- a/resources/input_pokemon.xlsx
+++ b/resources/input_pokemon.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonimm98\Desktop\ImagenesProyecto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonimm98\Documents\UiPath\pokemon-eoi\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16AB9303-7E97-4B93-B9F8-DB9F5FA5D5D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F96D52A-B7C5-4C76-A546-F2AAE498843E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13725" yWindow="2220" windowWidth="11385" windowHeight="11385" xr2:uid="{42483B01-2F9D-4BEA-A99A-B8C54C68AEFB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{42483B01-2F9D-4BEA-A99A-B8C54C68AEFB}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
   <si>
     <t>Pokemon</t>
   </si>
@@ -93,6 +93,9 @@
   </si>
   <si>
     <t>x</t>
+  </si>
+  <si>
+    <t>charmander</t>
   </si>
 </sst>
 </file>
@@ -447,7 +450,7 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -478,6 +481,9 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
       <c r="B3" t="s">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
cambio en la lógica, añadido el enviar email en el process transaction y envia por cada poekmon un excel porque no se crean las hojas KEK
</commit_message>
<xml_diff>
--- a/resources/input_pokemon.xlsx
+++ b/resources/input_pokemon.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonimm98\Documents\UiPath\pokemon-eoi\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F90DF6BA-A3A5-4972-9ECF-9D42167AF6C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1982331E-5C5A-4F3F-8162-FFA1F5EF8806}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14460" yWindow="1560" windowWidth="11385" windowHeight="11385" xr2:uid="{42483B01-2F9D-4BEA-A99A-B8C54C68AEFB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{42483B01-2F9D-4BEA-A99A-B8C54C68AEFB}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
   <si>
     <t>Pokemon</t>
   </si>
@@ -93,15 +93,6 @@
   </si>
   <si>
     <t>types</t>
-  </si>
-  <si>
-    <t>pikachu</t>
-  </si>
-  <si>
-    <t>chikorita</t>
-  </si>
-  <si>
-    <t>bulbasaur</t>
   </si>
 </sst>
 </file>
@@ -456,7 +447,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -498,9 +489,6 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>19</v>
-      </c>
       <c r="B4" t="s">
         <v>4</v>
       </c>
@@ -509,9 +497,6 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>20</v>
-      </c>
       <c r="B5" t="s">
         <v>18</v>
       </c>
@@ -520,9 +505,6 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>21</v>
-      </c>
       <c r="B6" t="s">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
robot funcional mas o menos
</commit_message>
<xml_diff>
--- a/resources/input_pokemon.xlsx
+++ b/resources/input_pokemon.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonimm98\Documents\UiPath\pokemon-eoi\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F6F6C3E-383C-44E0-B2DF-86045D1AB52F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19785100-4FE0-4F57-B6DD-6D8833B57FC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{42483B01-2F9D-4BEA-A99A-B8C54C68AEFB}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
   <si>
     <t>Pokemon</t>
   </si>
@@ -71,9 +71,6 @@
     <t>base_speed</t>
   </si>
   <si>
-    <t>sprite</t>
-  </si>
-  <si>
     <t>moves</t>
   </si>
   <si>
@@ -83,9 +80,6 @@
     <t>weight</t>
   </si>
   <si>
-    <t>totodile</t>
-  </si>
-  <si>
     <t>x</t>
   </si>
   <si>
@@ -95,10 +89,13 @@
     <t>types</t>
   </si>
   <si>
-    <t>charmander</t>
-  </si>
-  <si>
-    <t>pikachu</t>
+    <t>groudon</t>
+  </si>
+  <si>
+    <t>rayquaza</t>
+  </si>
+  <si>
+    <t>torchic</t>
   </si>
 </sst>
 </file>
@@ -450,10 +447,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F01141BE-88C1-41DE-8F4E-5B28F8D1A597}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -474,43 +471,43 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -548,25 +545,17 @@
         <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>12</v>
       </c>
-      <c r="C13" t="s">
-        <v>16</v>
-      </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>